<commit_message>
updated sample config files
</commit_message>
<xml_diff>
--- a/impact_analysis/data/impact_analysis_config_sample.xlsx
+++ b/impact_analysis/data/impact_analysis_config_sample.xlsx
@@ -2,16 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2" showHorizontalScroll="1" showVerticalScroll="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="mapping_column" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="segment" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="segment_columns" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="band" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
   </extLst>
@@ -19,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -39,6 +38,9 @@
     <t>Column</t>
   </si>
   <si>
+    <t>RNColumn</t>
+  </si>
+  <si>
     <t>POLICY_NUMBER</t>
   </si>
   <si>
@@ -60,6 +62,9 @@
     <t>data/input/file2.xlsx</t>
   </si>
   <si>
+    <t>PREMIUM_AMOUNT_Property_RN</t>
+  </si>
+  <si>
     <t>Inflation</t>
   </si>
   <si>
@@ -72,7 +77,34 @@
     <t>PREMIUM_AMOUNT_BI</t>
   </si>
   <si>
-    <t>Segment</t>
+    <t>PREMIUM_AMOUNT_BI_RN</t>
+  </si>
+  <si>
+    <t>ColumnToKeep</t>
+  </si>
+  <si>
+    <t>INCEPTION_DATE</t>
+  </si>
+  <si>
+    <t>EXPIRY_DATE</t>
+  </si>
+  <si>
+    <t>BUILDING_CONSTRUCTION_TYPE</t>
+  </si>
+  <si>
+    <t>OCCUPANCY_TYPE</t>
+  </si>
+  <si>
+    <t>BUILDING_AGE</t>
+  </si>
+  <si>
+    <t>LOCATION_CITY</t>
+  </si>
+  <si>
+    <t>LOCATION_STATE</t>
+  </si>
+  <si>
+    <t>RISK_CATEGORY</t>
   </si>
   <si>
     <t>From</t>
@@ -84,7 +116,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t xml:space="preserve">21.[99900%, Inf)</t>
+    <t>inf</t>
   </si>
 </sst>
 </file>
@@ -100,6 +132,8 @@
     </font>
     <font>
       <b/>
+      <sz val="11.000000"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -145,15 +179,15 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0"/>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="0" pivotButton="0">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -163,6 +197,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -673,21 +710,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
-  </sheetPr>
   <sheetViews>
     <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="18.7109375"/>
     <col customWidth="1" min="4" max="4" width="15.7109375"/>
-    <col customWidth="1" min="5" max="5" width="35.8515625"/>
-    <col bestFit="1" min="6" max="6" width="27.11328125"/>
+    <col customWidth="1" min="5" max="5" width="20.8515625"/>
+    <col customWidth="1" min="6" max="6" width="29.421875"/>
+    <col bestFit="1" customWidth="1" min="7" max="7" width="31.7109375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -709,127 +743,151 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>10</v>
+      <c r="G3" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2">
+        <v>17</v>
+      </c>
+      <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
+      <c r="D5" t="s">
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" ht="14.25">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="3">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25"/>
+    <row r="16" ht="14.25"/>
+    <row r="17" ht="14.25"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -840,23 +898,61 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
-  </sheetPr>
   <sheetViews>
     <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
-  <cols>
-    <col bestFit="1" customWidth="1" min="1" max="1" style="2" width="29.28125"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -869,29 +965,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
-  </sheetPr>
   <sheetViews>
     <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" min="3" max="3" style="2" width="18.00390625"/>
+    <col customWidth="1" min="3" max="3" width="18"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
@@ -903,13 +995,13 @@
         <v>-0.90000000000000002</v>
       </c>
       <c r="C2" t="str">
-        <f>_xlfn.CONCAT(ROW(A1),".[",TEXT(A2,"0%"),", ",TEXT(B2,"0%"),")")</f>
+        <f t="shared" ref="C2:C21" si="1">_xlfn.CONCAT(ROW(A1),".[",TEXT(A2,"0%"),", ",TEXT(B2,"0%"),")")</f>
         <v xml:space="preserve">1.[-100%, -90%)</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <f t="shared" ref="A3:A10" si="1">A2+0.1</f>
+        <f t="shared" ref="A3:A10" si="2">A2+0.1</f>
         <v>-0.90000000000000002</v>
       </c>
       <c r="B3">
@@ -917,13 +1009,13 @@
         <v>-0.80000000000000004</v>
       </c>
       <c r="C3" t="str">
-        <f>_xlfn.CONCAT(ROW(A2),".[",TEXT(A3,"0%"),", ",TEXT(B3,"0%"),")")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">2.[-90%, -80%)</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.80000000000000004</v>
       </c>
       <c r="B4">
@@ -931,13 +1023,13 @@
         <v>-0.70000000000000007</v>
       </c>
       <c r="C4" t="str">
-        <f>_xlfn.CONCAT(ROW(A3),".[",TEXT(A4,"0%"),", ",TEXT(B4,"0%"),")")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">3.[-80%, -70%)</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.70000000000000007</v>
       </c>
       <c r="B5">
@@ -945,13 +1037,13 @@
         <v>-0.60000000000000009</v>
       </c>
       <c r="C5" t="str">
-        <f>_xlfn.CONCAT(ROW(A4),".[",TEXT(A5,"0%"),", ",TEXT(B5,"0%"),")")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">4.[-70%, -60%)</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.60000000000000009</v>
       </c>
       <c r="B6">
@@ -959,13 +1051,13 @@
         <v>-0.50000000000000011</v>
       </c>
       <c r="C6" t="str">
-        <f>_xlfn.CONCAT(ROW(A5),".[",TEXT(A6,"0%"),", ",TEXT(B6,"0%"),")")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">5.[-60%, -50%)</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.50000000000000011</v>
       </c>
       <c r="B7">
@@ -973,13 +1065,13 @@
         <v>-0.40000000000000013</v>
       </c>
       <c r="C7" t="str">
-        <f>_xlfn.CONCAT(ROW(A6),".[",TEXT(A7,"0%"),", ",TEXT(B7,"0%"),")")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">6.[-50%, -40%)</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.40000000000000013</v>
       </c>
       <c r="B8">
@@ -987,35 +1079,35 @@
         <v>-0.30000000000000016</v>
       </c>
       <c r="C8" t="str">
-        <f>_xlfn.CONCAT(ROW(A7),".[",TEXT(A8,"0%"),", ",TEXT(B8,"0%"),")")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">7.[-40%, -30%)</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.30000000000000016</v>
       </c>
       <c r="B9">
-        <f t="shared" ref="B9:B21" si="2">A10</f>
+        <f t="shared" ref="B9:B20" si="3">A10</f>
         <v>-0.20000000000000015</v>
       </c>
       <c r="C9" t="str">
-        <f>_xlfn.CONCAT(ROW(A8),".[",TEXT(A9,"0%"),", ",TEXT(B9,"0%"),")")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">8.[-30%, -20%)</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.20000000000000015</v>
       </c>
       <c r="B10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.10000000000000014</v>
       </c>
       <c r="C10" t="str">
-        <f>_xlfn.CONCAT(ROW(A9),".[",TEXT(A10,"0%"),", ",TEXT(B10,"0%"),")")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">9.[-20%, -10%)</v>
       </c>
     </row>
@@ -1025,11 +1117,11 @@
         <v>-0.10000000000000014</v>
       </c>
       <c r="B11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C11" t="str">
-        <f>_xlfn.CONCAT(ROW(A10),".[",TEXT(A11,"0%"),", ",TEXT(B11,"0%"),")")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">10.[-10%, 0%)</v>
       </c>
     </row>
@@ -1038,81 +1130,81 @@
         <v>0</v>
       </c>
       <c r="B12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.10000000000000001</v>
       </c>
       <c r="C12" t="str">
-        <f>_xlfn.CONCAT(ROW(A11),".[",TEXT(A12,"0%"),", ",TEXT(B12,"0%"),")")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">11.[0%, 10%)</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <f t="shared" ref="A13:A17" si="3">A12+0.1</f>
+        <f t="shared" ref="A13:A17" si="4">A12+0.1</f>
         <v>0.10000000000000001</v>
       </c>
       <c r="B13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.20000000000000001</v>
       </c>
       <c r="C13" t="str">
-        <f>_xlfn.CONCAT(ROW(A12),".[",TEXT(A13,"0%"),", ",TEXT(B13,"0%"),")")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">12.[10%, 20%)</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
+        <f t="shared" si="4"/>
+        <v>0.20000000000000001</v>
+      </c>
+      <c r="B14">
         <f t="shared" si="3"/>
-        <v>0.20000000000000001</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="2"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="C14" t="str">
-        <f>_xlfn.CONCAT(ROW(A13),".[",TEXT(A14,"0%"),", ",TEXT(B14,"0%"),")")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">13.[20%, 30%)</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
+        <f t="shared" si="4"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="B15">
         <f t="shared" si="3"/>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="2"/>
         <v>0.40000000000000002</v>
       </c>
       <c r="C15" t="str">
-        <f>_xlfn.CONCAT(ROW(A14),".[",TEXT(A15,"0%"),", ",TEXT(B15,"0%"),")")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">14.[30%, 40%)</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
+        <f t="shared" si="4"/>
+        <v>0.40000000000000002</v>
+      </c>
+      <c r="B16">
         <f t="shared" si="3"/>
-        <v>0.40000000000000002</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="C16" t="str">
-        <f>_xlfn.CONCAT(ROW(A15),".[",TEXT(A16,"0%"),", ",TEXT(B16,"0%"),")")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">15.[40%, 50%)</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="B17">
         <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C17" t="str">
-        <f>_xlfn.CONCAT(ROW(A16),".[",TEXT(A17,"0%"),", ",TEXT(B17,"0%"),")")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">16.[50%, 100%)</v>
       </c>
     </row>
@@ -1121,11 +1213,11 @@
         <v>1</v>
       </c>
       <c r="B18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="C18" t="str">
-        <f>_xlfn.CONCAT(ROW(A17),".[",TEXT(A18,"0%"),", ",TEXT(B18,"0%"),")")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">17.[100%, 200%)</v>
       </c>
     </row>
@@ -1134,11 +1226,11 @@
         <v>2</v>
       </c>
       <c r="B19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="C19" t="str">
-        <f>_xlfn.CONCAT(ROW(A18),".[",TEXT(A19,"0%"),", ",TEXT(B19,"0%"),")")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">18.[200%, 500%)</v>
       </c>
     </row>
@@ -1147,11 +1239,11 @@
         <v>5</v>
       </c>
       <c r="B20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="C20" t="str">
-        <f>_xlfn.CONCAT(ROW(A19),".[",TEXT(A20,"0%"),", ",TEXT(B20,"0%"),")")</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve">19.[500%, 1000%)</v>
       </c>
     </row>
@@ -1159,21 +1251,12 @@
       <c r="A21">
         <v>10</v>
       </c>
-      <c r="B21">
-        <f t="shared" si="2"/>
-        <v>999</v>
+      <c r="B21" t="s">
+        <v>32</v>
       </c>
       <c r="C21" t="str">
-        <f>_xlfn.CONCAT(ROW(A20),".[",TEXT(A21,"0%"),", ",TEXT(B21,"0%"),")")</f>
-        <v xml:space="preserve">20.[1000%, 99900%)</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22">
-        <v>999</v>
-      </c>
-      <c r="C22" t="s">
-        <v>21</v>
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">20.[1000%, inf)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>